<commit_message>
Modified grid module and renamed functions
</commit_message>
<xml_diff>
--- a/tutorial/CovidContagion/data/input/grid_stay_prob.xlsx
+++ b/tutorial/CovidContagion/data/input/grid_stay_prob.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/ABM4ALL/Melodie/tutorial/CovidContagion/data/input/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CD7F71-C8F7-4D44-BEC4-13CD3F76F3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="30240" windowHeight="12980"/>
   </bookViews>
   <sheets>
     <sheet name="simulator_scenarios" sheetId="1" r:id="rId1"/>
@@ -20,25 +14,361 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -46,24 +376,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -321,23 +937,23 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:CV100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="35" workbookViewId="0">
-      <selection activeCell="AK57" sqref="AK57"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4"/>
   <sheetData>
-    <row r="1" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:100">
       <c r="A1">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -361,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="I1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J1">
         <v>0</v>
@@ -637,9 +1253,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:100">
       <c r="A2">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -939,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:100">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1241,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:100">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1543,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:100">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1845,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:100">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2147,7 +2763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:100">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2449,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:100">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2475,7 +3091,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -2751,7 +3367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:100">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3053,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:100">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3355,7 +3971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:100">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3657,7 +4273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:100">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3959,7 +4575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:100">
       <c r="A13">
         <v>0</v>
       </c>
@@ -4261,7 +4877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:100">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4563,7 +5179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:100">
       <c r="A15">
         <v>0</v>
       </c>
@@ -4865,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:100">
       <c r="A16">
         <v>0</v>
       </c>
@@ -5167,7 +5783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:100">
       <c r="A17">
         <v>0</v>
       </c>
@@ -5469,7 +6085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:100">
       <c r="A18">
         <v>0</v>
       </c>
@@ -5771,7 +6387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:100">
       <c r="A19">
         <v>0</v>
       </c>
@@ -6073,7 +6689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:100">
       <c r="A20">
         <v>0</v>
       </c>
@@ -6375,7 +6991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:100">
       <c r="A21">
         <v>0</v>
       </c>
@@ -6677,7 +7293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:100">
       <c r="A22">
         <v>0</v>
       </c>
@@ -6979,7 +7595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:100">
       <c r="A23">
         <v>0</v>
       </c>
@@ -7281,7 +7897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:100">
       <c r="A24">
         <v>0</v>
       </c>
@@ -7583,7 +8199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:100">
       <c r="A25">
         <v>0</v>
       </c>
@@ -7885,7 +8501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:100">
       <c r="A26">
         <v>0</v>
       </c>
@@ -8187,7 +8803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:100">
       <c r="A27">
         <v>0</v>
       </c>
@@ -8489,7 +9105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:100">
       <c r="A28">
         <v>0</v>
       </c>
@@ -8791,7 +9407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:100">
       <c r="A29">
         <v>0</v>
       </c>
@@ -9093,7 +9709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:100">
       <c r="A30">
         <v>0</v>
       </c>
@@ -9395,7 +10011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:100">
       <c r="A31">
         <v>0</v>
       </c>
@@ -9697,7 +10313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:100">
       <c r="A32">
         <v>0</v>
       </c>
@@ -9999,7 +10615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:100">
       <c r="A33">
         <v>0</v>
       </c>
@@ -10301,7 +10917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:100">
       <c r="A34">
         <v>0</v>
       </c>
@@ -10603,7 +11219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:100">
       <c r="A35">
         <v>0</v>
       </c>
@@ -10905,7 +11521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:100">
       <c r="A36">
         <v>0</v>
       </c>
@@ -11207,7 +11823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:100">
       <c r="A37">
         <v>0</v>
       </c>
@@ -11509,7 +12125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:100">
       <c r="A38">
         <v>0</v>
       </c>
@@ -11811,7 +12427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:100">
       <c r="A39">
         <v>0</v>
       </c>
@@ -12113,7 +12729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:100">
       <c r="A40">
         <v>0</v>
       </c>
@@ -12415,7 +13031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:100">
       <c r="A41">
         <v>0</v>
       </c>
@@ -12717,7 +13333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:100">
       <c r="A42">
         <v>0</v>
       </c>
@@ -13019,7 +13635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:100">
       <c r="A43">
         <v>0</v>
       </c>
@@ -13321,7 +13937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:100">
       <c r="A44">
         <v>0</v>
       </c>
@@ -13623,7 +14239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:100">
       <c r="A45">
         <v>0</v>
       </c>
@@ -13925,7 +14541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:100">
       <c r="A46">
         <v>0</v>
       </c>
@@ -14227,7 +14843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:100">
       <c r="A47">
         <v>0</v>
       </c>
@@ -14529,7 +15145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:100">
       <c r="A48">
         <v>0</v>
       </c>
@@ -14831,7 +15447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:100">
       <c r="A49">
         <v>0</v>
       </c>
@@ -15133,7 +15749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:100">
       <c r="A50">
         <v>0</v>
       </c>
@@ -15435,7 +16051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:100">
       <c r="A51">
         <v>0</v>
       </c>
@@ -15737,7 +16353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:100">
       <c r="A52">
         <v>0</v>
       </c>
@@ -16039,7 +16655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:100">
       <c r="A53">
         <v>0</v>
       </c>
@@ -16341,7 +16957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:100">
       <c r="A54">
         <v>0</v>
       </c>
@@ -16643,7 +17259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:100">
       <c r="A55">
         <v>0</v>
       </c>
@@ -16945,7 +17561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:100">
       <c r="A56">
         <v>0</v>
       </c>
@@ -17247,7 +17863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:100">
       <c r="A57">
         <v>0</v>
       </c>
@@ -17549,7 +18165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:100">
       <c r="A58">
         <v>0</v>
       </c>
@@ -17851,7 +18467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:100">
       <c r="A59">
         <v>0</v>
       </c>
@@ -18153,7 +18769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:100">
       <c r="A60">
         <v>0</v>
       </c>
@@ -18455,7 +19071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:100">
       <c r="A61">
         <v>0</v>
       </c>
@@ -18757,7 +19373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:100">
       <c r="A62">
         <v>0</v>
       </c>
@@ -19059,7 +19675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:100">
       <c r="A63">
         <v>0</v>
       </c>
@@ -19361,7 +19977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:100">
       <c r="A64">
         <v>0</v>
       </c>
@@ -19663,7 +20279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:100">
       <c r="A65">
         <v>0</v>
       </c>
@@ -19965,7 +20581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:100">
       <c r="A66">
         <v>0</v>
       </c>
@@ -20267,7 +20883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:100">
       <c r="A67">
         <v>0</v>
       </c>
@@ -20569,7 +21185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:100">
       <c r="A68">
         <v>0</v>
       </c>
@@ -20871,7 +21487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:100">
       <c r="A69">
         <v>0</v>
       </c>
@@ -21173,7 +21789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:100">
       <c r="A70">
         <v>0</v>
       </c>
@@ -21475,7 +22091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:100">
       <c r="A71">
         <v>0</v>
       </c>
@@ -21777,7 +22393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:100">
       <c r="A72">
         <v>0</v>
       </c>
@@ -22079,7 +22695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:100">
       <c r="A73">
         <v>0</v>
       </c>
@@ -22381,7 +22997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:100">
       <c r="A74">
         <v>0</v>
       </c>
@@ -22683,7 +23299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:100">
       <c r="A75">
         <v>0</v>
       </c>
@@ -22985,7 +23601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:100">
       <c r="A76">
         <v>0</v>
       </c>
@@ -23287,7 +23903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:100">
       <c r="A77">
         <v>0</v>
       </c>
@@ -23589,7 +24205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:100">
       <c r="A78">
         <v>0</v>
       </c>
@@ -23891,7 +24507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:100">
       <c r="A79">
         <v>0</v>
       </c>
@@ -24193,7 +24809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:100">
       <c r="A80">
         <v>0</v>
       </c>
@@ -24495,7 +25111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:100">
       <c r="A81">
         <v>0</v>
       </c>
@@ -24797,7 +25413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:100">
       <c r="A82">
         <v>0</v>
       </c>
@@ -25099,7 +25715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:100">
       <c r="A83">
         <v>0</v>
       </c>
@@ -25401,7 +26017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:100">
       <c r="A84">
         <v>0</v>
       </c>
@@ -25703,7 +26319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:100">
       <c r="A85">
         <v>0</v>
       </c>
@@ -26005,7 +26621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:100">
       <c r="A86">
         <v>0</v>
       </c>
@@ -26307,7 +26923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:100">
       <c r="A87">
         <v>0</v>
       </c>
@@ -26609,7 +27225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:100">
       <c r="A88">
         <v>0</v>
       </c>
@@ -26911,7 +27527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:100">
       <c r="A89">
         <v>0</v>
       </c>
@@ -27213,7 +27829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:100">
       <c r="A90">
         <v>0</v>
       </c>
@@ -27515,7 +28131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:100">
       <c r="A91">
         <v>0</v>
       </c>
@@ -27817,7 +28433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:100">
       <c r="A92">
         <v>0</v>
       </c>
@@ -28119,7 +28735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:100">
       <c r="A93">
         <v>0</v>
       </c>
@@ -28421,7 +29037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:100">
       <c r="A94">
         <v>0</v>
       </c>
@@ -28723,7 +29339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:100">
       <c r="A95">
         <v>0</v>
       </c>
@@ -29025,7 +29641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:100">
       <c r="A96">
         <v>0</v>
       </c>
@@ -29327,7 +29943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:100">
       <c r="A97">
         <v>0</v>
       </c>
@@ -29629,7 +30245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:100">
       <c r="A98">
         <v>0</v>
       </c>
@@ -29931,7 +30547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:100">
       <c r="A99">
         <v>0</v>
       </c>
@@ -30233,7 +30849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:100">
       <c r="A100">
         <v>0</v>
       </c>
@@ -30538,5 +31154,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>